<commit_message>
Add brand partnership growth parameters: initial brands + quarterly growth rate with revenue impact calculations
</commit_message>
<xml_diff>
--- a/brand/kshipra_commerce_reward_model.xlsx
+++ b/brand/kshipra_commerce_reward_model.xlsx
@@ -162,8 +162,8 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="3" fontId="3" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="1" fontId="3" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="1" fontId="3" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1027,7 +1027,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1098,333 +1098,333 @@
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>AD ECONOMICS</t>
+          <t>BRAND PARTNERSHIP GROWTH</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>CPV - Brand Pays per View</t>
-        </is>
-      </c>
-      <c r="B8" s="9" t="n">
-        <v>0.2</v>
+          <t>Initial Brands Enrolled</t>
+        </is>
+      </c>
+      <c r="B8" s="11" t="n">
+        <v>10</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>$</t>
+          <t>brands</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Revenue per verified ad view (100% engagement)</t>
+          <t>Starting number of brand advertisers</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>Quarterly Brand Growth Rate</t>
+        </is>
+      </c>
+      <c r="B9" s="12" t="n">
+        <v>25</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>% increase in brands each quarter (compounding)</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>AD ECONOMICS</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>CPV - Brand Pays per View</t>
+        </is>
+      </c>
+      <c r="B12" s="9" t="n">
+        <v>0.2</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Revenue per verified ad view (100% engagement)</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
           <t>Cash Credit per View</t>
         </is>
       </c>
-      <c r="B9" s="9" t="n">
+      <c r="B13" s="9" t="n">
         <v>0.06</v>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C13" t="inlineStr">
         <is>
           <t>$</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D13" t="inlineStr">
         <is>
           <t>Instant cash reward to user (goes to wallet)</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>Reward Points per View</t>
-        </is>
-      </c>
-      <c r="B10" s="9" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>$</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Store credit reward (redeemable at partner stores)</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Kshipra Margin per View</t>
-        </is>
-      </c>
-      <c r="B11" s="9" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>$</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Our profit per ad = CPV - Cash - Rewards</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="inlineStr">
-        <is>
-          <t>USER ENGAGEMENT</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Active User Rate</t>
-        </is>
-      </c>
-      <c r="B14" s="11" t="n">
-        <v>60</v>
+          <t>Reward Points per View</t>
+        </is>
+      </c>
+      <c r="B14" s="9" t="n">
+        <v>0.06</v>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>%</t>
+          <t>$</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>% of buyers who actually watch ads to earn rewards</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="inlineStr">
-        <is>
-          <t>USER BEHAVIOR</t>
+          <t>Store credit reward (redeemable at partner stores)</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Kshipra Margin per View</t>
+        </is>
+      </c>
+      <c r="B15" s="9" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Our profit per ad = CPV - Cash - Rewards</t>
         </is>
       </c>
     </row>
     <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>Avg Ads to Recover Bag Cost</t>
-        </is>
-      </c>
-      <c r="B17" s="12" t="n">
-        <v>3</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>ads</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>How many ads needed to make bag FREE</t>
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>USER ENGAGEMENT</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Avg Monthly Ad Views per User</t>
+          <t>Active User Rate</t>
         </is>
       </c>
       <c r="B18" s="12" t="n">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>views</t>
+          <t>%</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Engagement level: ads watched per active user/month</t>
+          <t>% of buyers who actually watch ads to earn rewards</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="inlineStr">
         <is>
-          <t>TIER CASH CREDIT LIMITS</t>
+          <t>USER BEHAVIOR</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Bronze - Bag Values/Month</t>
+          <t>Avg Ads to Recover Bag Cost</t>
         </is>
       </c>
       <c r="B21" s="11" t="n">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>ads</t>
+        </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Low-engagement: 1 bag purchase/month</t>
+          <t>How many ads needed to make bag FREE</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>Avg Monthly Ad Views per User</t>
+        </is>
+      </c>
+      <c r="B22" s="11" t="n">
+        <v>12</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>views</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>Engagement level: ads watched per active user/month</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>TIER CASH CREDIT LIMITS</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Bronze - Bag Values/Month</t>
+        </is>
+      </c>
+      <c r="B25" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>Low-engagement: 1 bag purchase/month</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
           <t>Silver - Bag Values/Month</t>
         </is>
       </c>
-      <c r="B22" s="11" t="n">
+      <c r="B26" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="D26" t="inlineStr">
         <is>
           <t>Medium-engagement: 3 bags/month</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Gold - Bag Values/Month</t>
-        </is>
-      </c>
-      <c r="B23" s="11" t="n">
-        <v>7</v>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>High-engagement: 7 bags/month</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Platinum - Daily Cap ($)</t>
-        </is>
-      </c>
-      <c r="B24" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Super users: $1/day earning limit</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="2" t="inlineStr">
-        <is>
-          <t>USER DISTRIBUTION BY TIER (%)</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Bronze %</t>
-        </is>
-      </c>
-      <c r="B27" s="11" t="n">
-        <v>60</v>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>%</t>
-        </is>
+          <t>Gold - Bag Values/Month</t>
+        </is>
+      </c>
+      <c r="B27" s="12" t="n">
+        <v>7</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>Most users are casual shoppers</t>
+          <t>High-engagement: 7 bags/month</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
+          <t>Platinum - Daily Cap ($)</t>
+        </is>
+      </c>
+      <c r="B28" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Super users: $1/day earning limit</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="inlineStr">
+        <is>
+          <t>USER DISTRIBUTION BY TIER (%)</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Bronze %</t>
+        </is>
+      </c>
+      <c r="B31" s="12" t="n">
+        <v>60</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Most users are casual shoppers</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
           <t>Silver %</t>
         </is>
       </c>
-      <c r="B28" s="11" t="n">
+      <c r="B32" s="12" t="n">
         <v>25</v>
       </c>
-      <c r="C28" t="inlineStr">
+      <c r="C32" t="inlineStr">
         <is>
           <t>%</t>
         </is>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="D32" t="inlineStr">
         <is>
           <t>Regular shoppers</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>Gold %</t>
-        </is>
-      </c>
-      <c r="B29" s="11" t="n">
-        <v>12</v>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>%</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>Frequent shoppers</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Platinum %</t>
-        </is>
-      </c>
-      <c r="B30" s="11" t="n">
-        <v>3</v>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>%</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>Power users (heavy engagement)</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" s="2" t="inlineStr">
-        <is>
-          <t>STORE &amp; REDEMPTION METRICS</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Reward Redemption Rate</t>
-        </is>
-      </c>
-      <c r="B33" s="11" t="n">
-        <v>75</v>
+          <t>Gold %</t>
+        </is>
+      </c>
+      <c r="B33" s="12" t="n">
+        <v>12</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1433,148 +1433,196 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>% of users who redeem rewards at stores</t>
+          <t>Frequent shoppers</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>Platinum %</t>
+        </is>
+      </c>
+      <c r="B34" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Power users (heavy engagement)</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="inlineStr">
+        <is>
+          <t>STORE &amp; REDEMPTION METRICS</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Reward Redemption Rate</t>
+        </is>
+      </c>
+      <c r="B37" s="12" t="n">
+        <v>75</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>% of users who redeem rewards at stores</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
           <t>Repeat Visit Increase</t>
         </is>
       </c>
-      <c r="B34" s="11" t="n">
+      <c r="B38" s="12" t="n">
         <v>15</v>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="C38" t="inlineStr">
         <is>
           <t>%</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="D38" t="inlineStr">
         <is>
           <t>Users visit more often to use rewards</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>Basket Size Uplift</t>
-        </is>
-      </c>
-      <c r="B35" s="11" t="n">
-        <v>8</v>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>%</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>Users buy more when they have rewards</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>Average Basket Value</t>
-        </is>
-      </c>
-      <c r="B36" s="9" t="n">
-        <v>25</v>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>$</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>Typical purchase amount per store visit</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" s="2" t="inlineStr">
-        <is>
-          <t>BRAND BENCHMARKS</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Meta CPM</t>
-        </is>
-      </c>
-      <c r="B39" s="9" t="n">
-        <v>10</v>
+          <t>Basket Size Uplift</t>
+        </is>
+      </c>
+      <c r="B39" s="12" t="n">
+        <v>8</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>$</t>
+          <t>%</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Facebook/Instagram ad cost per 1000 impressions</t>
+          <t>Users buy more when they have rewards</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
+          <t>Average Basket Value</t>
+        </is>
+      </c>
+      <c r="B40" s="9" t="n">
+        <v>25</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Typical purchase amount per store visit</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="inlineStr">
+        <is>
+          <t>BRAND BENCHMARKS</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Meta CPM</t>
+        </is>
+      </c>
+      <c r="B43" s="9" t="n">
+        <v>10</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Facebook/Instagram ad cost per 1000 impressions</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
           <t>TikTok CPM</t>
         </is>
       </c>
-      <c r="B40" s="9" t="n">
+      <c r="B44" s="9" t="n">
         <v>8.5</v>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="C44" t="inlineStr">
         <is>
           <t>$</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="D44" t="inlineStr">
         <is>
           <t>TikTok ad cost per 1000 impressions</t>
         </is>
       </c>
     </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
+    <row r="45">
+      <c r="A45" t="inlineStr">
         <is>
           <t>Industry Avg CTR</t>
         </is>
       </c>
-      <c r="B41" s="11" t="n">
+      <c r="B45" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="C41" t="inlineStr">
+      <c r="C45" t="inlineStr">
         <is>
           <t>%</t>
         </is>
       </c>
-      <c r="D41" t="inlineStr">
+      <c r="D45" t="inlineStr">
         <is>
           <t>Click-through rate on social media ads (only 1% engage!)</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="10">
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A17:D17"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A26:D26"/>
-    <mergeCell ref="A38:D38"/>
+    <mergeCell ref="A30:D30"/>
     <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A16:D16"/>
-    <mergeCell ref="A32:D32"/>
-    <mergeCell ref="A13:D13"/>
+    <mergeCell ref="A24:D24"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A36:D36"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1636,7 +1684,7 @@
         </is>
       </c>
       <c r="B5" s="14">
-        <f>Assumptions!B5*Assumptions!B14/100</f>
+        <f>Assumptions!B5*Assumptions!B18/100</f>
         <v/>
       </c>
       <c r="C5" t="inlineStr">
@@ -1668,7 +1716,7 @@
         </is>
       </c>
       <c r="B7" s="14">
-        <f>B5*Assumptions!B18</f>
+        <f>B5*Assumptions!B22</f>
         <v/>
       </c>
       <c r="C7" t="inlineStr">
@@ -1684,7 +1732,7 @@
         </is>
       </c>
       <c r="B8" s="15">
-        <f>B7*Assumptions!B8</f>
+        <f>B7*Assumptions!B12</f>
         <v/>
       </c>
       <c r="C8" t="inlineStr">
@@ -1716,7 +1764,7 @@
         </is>
       </c>
       <c r="B11" s="15">
-        <f>B7*Assumptions!B9</f>
+        <f>B7*Assumptions!B13</f>
         <v/>
       </c>
       <c r="C11" t="inlineStr">
@@ -1732,7 +1780,7 @@
         </is>
       </c>
       <c r="B12" s="15">
-        <f>B7*Assumptions!B10</f>
+        <f>B7*Assumptions!B14</f>
         <v/>
       </c>
       <c r="C12" t="inlineStr">
@@ -1748,7 +1796,7 @@
         </is>
       </c>
       <c r="B13" s="15">
-        <f>B7*Assumptions!B11</f>
+        <f>B7*Assumptions!B15</f>
         <v/>
       </c>
       <c r="C13" t="inlineStr">
@@ -1803,7 +1851,7 @@
         </is>
       </c>
       <c r="B18">
-        <f>Assumptions!B18</f>
+        <f>Assumptions!B22</f>
         <v/>
       </c>
       <c r="C18" t="inlineStr">
@@ -1819,7 +1867,7 @@
         </is>
       </c>
       <c r="B19" s="19">
-        <f>Assumptions!B18*Assumptions!B8</f>
+        <f>Assumptions!B22*Assumptions!B12</f>
         <v/>
       </c>
       <c r="C19" t="inlineStr">
@@ -1835,7 +1883,7 @@
         </is>
       </c>
       <c r="B20" s="19">
-        <f>Assumptions!B18*(Assumptions!B9+Assumptions!B10)</f>
+        <f>Assumptions!B22*(Assumptions!B13+Assumptions!B14)</f>
         <v/>
       </c>
       <c r="C20" t="inlineStr">
@@ -1851,7 +1899,7 @@
         </is>
       </c>
       <c r="B21" s="19">
-        <f>Assumptions!B18*Assumptions!B11</f>
+        <f>Assumptions!B22*Assumptions!B15</f>
         <v/>
       </c>
       <c r="C21" t="inlineStr">
@@ -1890,7 +1938,7 @@
         </is>
       </c>
       <c r="B25">
-        <f>Assumptions!B17</f>
+        <f>Assumptions!B21</f>
         <v/>
       </c>
       <c r="C25" t="inlineStr">
@@ -1906,7 +1954,7 @@
         </is>
       </c>
       <c r="B26" s="19">
-        <f>Assumptions!B17*Assumptions!B8</f>
+        <f>Assumptions!B21*Assumptions!B12</f>
         <v/>
       </c>
       <c r="C26" t="inlineStr">
@@ -1922,7 +1970,7 @@
         </is>
       </c>
       <c r="B27" s="19">
-        <f>Assumptions!B17*(Assumptions!B9+Assumptions!B10)</f>
+        <f>Assumptions!B21*(Assumptions!B13+Assumptions!B14)</f>
         <v/>
       </c>
       <c r="C27" t="inlineStr">
@@ -1961,7 +2009,7 @@
         </is>
       </c>
       <c r="B31" s="15">
-        <f>B7*(Assumptions!B9+Assumptions!B10)</f>
+        <f>B7*(Assumptions!B13+Assumptions!B14)</f>
         <v/>
       </c>
       <c r="C31" t="inlineStr">
@@ -1977,7 +2025,7 @@
         </is>
       </c>
       <c r="B32" s="15">
-        <f>B31*Assumptions!B33/100</f>
+        <f>B31*Assumptions!B37/100</f>
         <v/>
       </c>
       <c r="C32" t="inlineStr">
@@ -1993,7 +2041,7 @@
         </is>
       </c>
       <c r="B33" s="14">
-        <f>Assumptions!B5*Assumptions!B33/100</f>
+        <f>Assumptions!B5*Assumptions!B37/100</f>
         <v/>
       </c>
       <c r="C33" t="inlineStr">
@@ -2009,7 +2057,7 @@
         </is>
       </c>
       <c r="B34" s="15">
-        <f>B33*Assumptions!B36</f>
+        <f>B33*Assumptions!B40</f>
         <v/>
       </c>
       <c r="C34" t="inlineStr">
@@ -2025,7 +2073,7 @@
         </is>
       </c>
       <c r="B35" s="15">
-        <f>B34*Assumptions!B35/100</f>
+        <f>B34*Assumptions!B39/100</f>
         <v/>
       </c>
       <c r="C35" t="inlineStr">
@@ -2055,7 +2103,7 @@
         </is>
       </c>
       <c r="B39" s="19">
-        <f>Assumptions!B8*1000</f>
+        <f>Assumptions!B12*1000</f>
         <v/>
       </c>
       <c r="C39" t="inlineStr">
@@ -2071,7 +2119,7 @@
         </is>
       </c>
       <c r="B40" s="19">
-        <f>Assumptions!B8</f>
+        <f>Assumptions!B12</f>
         <v/>
       </c>
       <c r="C40" t="inlineStr">
@@ -2110,7 +2158,7 @@
         </is>
       </c>
       <c r="B44" s="19">
-        <f>Assumptions!B39</f>
+        <f>Assumptions!B43</f>
         <v/>
       </c>
       <c r="C44" t="inlineStr">
@@ -2126,7 +2174,7 @@
         </is>
       </c>
       <c r="B45" s="23">
-        <f>Assumptions!B41</f>
+        <f>Assumptions!B45</f>
         <v/>
       </c>
       <c r="C45" t="inlineStr">
@@ -2142,7 +2190,7 @@
         </is>
       </c>
       <c r="B46" s="19">
-        <f>(Assumptions!B39/1000)/(Assumptions!B41/100)</f>
+        <f>(Assumptions!B43/1000)/(Assumptions!B45/100)</f>
         <v/>
       </c>
       <c r="C46" t="inlineStr">
@@ -2578,7 +2626,7 @@
           <t>Avg User Lifetime (months)</t>
         </is>
       </c>
-      <c r="B5" s="11" t="n">
+      <c r="B5" s="12" t="n">
         <v>12</v>
       </c>
       <c r="C5" t="inlineStr">
@@ -2617,7 +2665,7 @@
         </is>
       </c>
       <c r="B9" s="19">
-        <f>B5*Assumptions!B18*Assumptions!B11</f>
+        <f>B5*Assumptions!B22*Assumptions!B15</f>
         <v/>
       </c>
       <c r="C9" t="inlineStr">
@@ -2672,7 +2720,7 @@
         </is>
       </c>
       <c r="B14" s="19">
-        <f>(Assumptions!B4)+(Assumptions!B18*Assumptions!B11)</f>
+        <f>(Assumptions!B4)+(Assumptions!B22*Assumptions!B15)</f>
         <v/>
       </c>
       <c r="C14" t="inlineStr">
@@ -2743,7 +2791,7 @@
         </is>
       </c>
       <c r="B20" s="27">
-        <f>Calculations!B33*12*Assumptions!B36*1.15</f>
+        <f>Calculations!B33*12*Assumptions!B40*1.15</f>
         <v/>
       </c>
       <c r="C20" t="inlineStr">
@@ -3478,7 +3526,7 @@
         </is>
       </c>
       <c r="B22" s="19">
-        <f>-Assumptions!B17*Assumptions!B9</f>
+        <f>-Assumptions!B21*Assumptions!B13</f>
         <v/>
       </c>
       <c r="C22" t="inlineStr">
@@ -3494,7 +3542,7 @@
         </is>
       </c>
       <c r="B23" s="19">
-        <f>-Assumptions!B17*Assumptions!B10</f>
+        <f>-Assumptions!B21*Assumptions!B14</f>
         <v/>
       </c>
       <c r="C23" t="inlineStr">
@@ -3555,7 +3603,7 @@
         </is>
       </c>
       <c r="B39" s="33">
-        <f>(12*(Assumptions!B4+Assumptions!B18*Assumptions!B11))/2</f>
+        <f>(12*(Assumptions!B4+Assumptions!B22*Assumptions!B15))/2</f>
         <v/>
       </c>
       <c r="C39" t="inlineStr">
@@ -3576,7 +3624,7 @@
         </is>
       </c>
       <c r="B40" s="34">
-        <f>2/(Assumptions!B4+Assumptions!B18*Assumptions!B11)</f>
+        <f>2/(Assumptions!B4+Assumptions!B22*Assumptions!B15)</f>
         <v/>
       </c>
       <c r="C40" t="inlineStr">
@@ -3637,7 +3685,7 @@
         </is>
       </c>
       <c r="B45" s="27">
-        <f>Calculations!B31*Assumptions!B33/100</f>
+        <f>Calculations!B31*Assumptions!B37/100</f>
         <v/>
       </c>
       <c r="C45" t="inlineStr">
@@ -3669,7 +3717,7 @@
         </is>
       </c>
       <c r="B47" s="27">
-        <f>Calculations!B34*Assumptions!B35/100</f>
+        <f>Calculations!B34*Assumptions!B39/100</f>
         <v/>
       </c>
       <c r="C47" t="inlineStr">

</xml_diff>

<commit_message>
Add quarterly bag sales growth parameter (15%) - combined with brand growth creates 29.4% total revenue lift in Year 1
</commit_message>
<xml_diff>
--- a/brand/kshipra_commerce_reward_model.xlsx
+++ b/brand/kshipra_commerce_reward_model.xlsx
@@ -162,8 +162,8 @@
     </xf>
     <xf numFmtId="164" fontId="3" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="3" fontId="3" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="1" fontId="3" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1027,7 +1027,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1091,92 +1091,92 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Monthly volume - scale this to model growth</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="inlineStr">
+          <t>Initial monthly volume - will grow quarterly</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Quarterly Bag Sales Growth</t>
+        </is>
+      </c>
+      <c r="B6" s="11" t="n">
+        <v>15</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>% increase in bag sales each quarter (compounding)</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="inlineStr">
         <is>
           <t>BRAND PARTNERSHIP GROWTH</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Initial Brands Enrolled</t>
-        </is>
-      </c>
-      <c r="B8" s="11" t="n">
-        <v>10</v>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>brands</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Starting number of brand advertisers</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>Initial Brands Enrolled</t>
+        </is>
+      </c>
+      <c r="B9" s="12" t="n">
+        <v>10</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>brands</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>Starting number of brand advertisers</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
           <t>Quarterly Brand Growth Rate</t>
         </is>
       </c>
-      <c r="B9" s="12" t="n">
+      <c r="B10" s="11" t="n">
         <v>25</v>
       </c>
-      <c r="C9" t="inlineStr">
+      <c r="C10" t="inlineStr">
         <is>
           <t>%</t>
         </is>
       </c>
-      <c r="D9" t="inlineStr">
+      <c r="D10" t="inlineStr">
         <is>
           <t>% increase in brands each quarter (compounding)</t>
         </is>
       </c>
     </row>
-    <row r="11">
-      <c r="A11" s="2" t="inlineStr">
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
         <is>
           <t>AD ECONOMICS</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>CPV - Brand Pays per View</t>
-        </is>
-      </c>
-      <c r="B12" s="9" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>$</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Revenue per verified ad view (100% engagement)</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Cash Credit per View</t>
+          <t>CPV - Brand Pays per View</t>
         </is>
       </c>
       <c r="B13" s="9" t="n">
-        <v>0.06</v>
+        <v>0.2</v>
       </c>
       <c r="C13" t="inlineStr">
         <is>
@@ -1185,14 +1185,14 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>Instant cash reward to user (goes to wallet)</t>
+          <t>Revenue per verified ad view (100% engagement)</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Reward Points per View</t>
+          <t>Cash Credit per View</t>
         </is>
       </c>
       <c r="B14" s="9" t="n">
@@ -1205,206 +1205,206 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>Store credit reward (redeemable at partner stores)</t>
+          <t>Instant cash reward to user (goes to wallet)</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>Reward Points per View</t>
+        </is>
+      </c>
+      <c r="B15" s="9" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Store credit reward (redeemable at partner stores)</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
           <t>Kshipra Margin per View</t>
         </is>
       </c>
-      <c r="B15" s="9" t="n">
+      <c r="B16" s="9" t="n">
         <v>0.08</v>
       </c>
-      <c r="C15" t="inlineStr">
+      <c r="C16" t="inlineStr">
         <is>
           <t>$</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>Our profit per ad = CPV - Cash - Rewards</t>
         </is>
       </c>
     </row>
-    <row r="17">
-      <c r="A17" s="2" t="inlineStr">
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
         <is>
           <t>USER ENGAGEMENT</t>
         </is>
       </c>
     </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
+    <row r="19">
+      <c r="A19" t="inlineStr">
         <is>
           <t>Active User Rate</t>
         </is>
       </c>
-      <c r="B18" s="12" t="n">
+      <c r="B19" s="11" t="n">
         <v>60</v>
       </c>
-      <c r="C18" t="inlineStr">
+      <c r="C19" t="inlineStr">
         <is>
           <t>%</t>
         </is>
       </c>
-      <c r="D18" t="inlineStr">
+      <c r="D19" t="inlineStr">
         <is>
           <t>% of buyers who actually watch ads to earn rewards</t>
         </is>
       </c>
     </row>
-    <row r="20">
-      <c r="A20" s="2" t="inlineStr">
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
         <is>
           <t>USER BEHAVIOR</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
-        <is>
-          <t>Avg Ads to Recover Bag Cost</t>
-        </is>
-      </c>
-      <c r="B21" s="11" t="n">
-        <v>3</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>ads</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>How many ads needed to make bag FREE</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>Avg Ads to Recover Bag Cost</t>
+        </is>
+      </c>
+      <c r="B22" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>ads</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>How many ads needed to make bag FREE</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
           <t>Avg Monthly Ad Views per User</t>
         </is>
       </c>
-      <c r="B22" s="11" t="n">
+      <c r="B23" s="12" t="n">
         <v>12</v>
       </c>
-      <c r="C22" t="inlineStr">
+      <c r="C23" t="inlineStr">
         <is>
           <t>views</t>
         </is>
       </c>
-      <c r="D22" t="inlineStr">
+      <c r="D23" t="inlineStr">
         <is>
           <t>Engagement level: ads watched per active user/month</t>
         </is>
       </c>
     </row>
-    <row r="24">
-      <c r="A24" s="2" t="inlineStr">
+    <row r="25">
+      <c r="A25" s="2" t="inlineStr">
         <is>
           <t>TIER CASH CREDIT LIMITS</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Bronze - Bag Values/Month</t>
-        </is>
-      </c>
-      <c r="B25" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>Low-engagement: 1 bag purchase/month</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Silver - Bag Values/Month</t>
-        </is>
-      </c>
-      <c r="B26" s="12" t="n">
-        <v>3</v>
+          <t>Bronze - Bag Values/Month</t>
+        </is>
+      </c>
+      <c r="B26" s="11" t="n">
+        <v>1</v>
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>Medium-engagement: 3 bags/month</t>
+          <t>Low-engagement: 1 bag purchase/month</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Gold - Bag Values/Month</t>
-        </is>
-      </c>
-      <c r="B27" s="12" t="n">
-        <v>7</v>
+          <t>Silver - Bag Values/Month</t>
+        </is>
+      </c>
+      <c r="B27" s="11" t="n">
+        <v>3</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>High-engagement: 7 bags/month</t>
+          <t>Medium-engagement: 3 bags/month</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
+          <t>Gold - Bag Values/Month</t>
+        </is>
+      </c>
+      <c r="B28" s="11" t="n">
+        <v>7</v>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>High-engagement: 7 bags/month</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
           <t>Platinum - Daily Cap ($)</t>
         </is>
       </c>
-      <c r="B28" s="9" t="n">
+      <c r="B29" s="9" t="n">
         <v>1</v>
       </c>
-      <c r="D28" t="inlineStr">
+      <c r="D29" t="inlineStr">
         <is>
           <t>Super users: $1/day earning limit</t>
         </is>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" s="2" t="inlineStr">
+    <row r="31">
+      <c r="A31" s="2" t="inlineStr">
         <is>
           <t>USER DISTRIBUTION BY TIER (%)</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Bronze %</t>
-        </is>
-      </c>
-      <c r="B31" s="12" t="n">
-        <v>60</v>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>%</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>Most users are casual shoppers</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Silver %</t>
-        </is>
-      </c>
-      <c r="B32" s="12" t="n">
-        <v>25</v>
+          <t>Bronze %</t>
+        </is>
+      </c>
+      <c r="B32" s="11" t="n">
+        <v>60</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
@@ -1413,18 +1413,18 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Regular shoppers</t>
+          <t>Most users are casual shoppers</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Gold %</t>
-        </is>
-      </c>
-      <c r="B33" s="12" t="n">
-        <v>12</v>
+          <t>Silver %</t>
+        </is>
+      </c>
+      <c r="B33" s="11" t="n">
+        <v>25</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
@@ -1433,65 +1433,65 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>Frequent shoppers</t>
+          <t>Regular shoppers</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
+          <t>Gold %</t>
+        </is>
+      </c>
+      <c r="B34" s="11" t="n">
+        <v>12</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Frequent shoppers</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
           <t>Platinum %</t>
         </is>
       </c>
-      <c r="B34" s="12" t="n">
+      <c r="B35" s="11" t="n">
         <v>3</v>
       </c>
-      <c r="C34" t="inlineStr">
+      <c r="C35" t="inlineStr">
         <is>
           <t>%</t>
         </is>
       </c>
-      <c r="D34" t="inlineStr">
+      <c r="D35" t="inlineStr">
         <is>
           <t>Power users (heavy engagement)</t>
         </is>
       </c>
     </row>
-    <row r="36">
-      <c r="A36" s="2" t="inlineStr">
+    <row r="37">
+      <c r="A37" s="2" t="inlineStr">
         <is>
           <t>STORE &amp; REDEMPTION METRICS</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>Reward Redemption Rate</t>
-        </is>
-      </c>
-      <c r="B37" s="12" t="n">
-        <v>75</v>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>%</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>% of users who redeem rewards at stores</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Repeat Visit Increase</t>
-        </is>
-      </c>
-      <c r="B38" s="12" t="n">
-        <v>15</v>
+          <t>Reward Redemption Rate</t>
+        </is>
+      </c>
+      <c r="B38" s="11" t="n">
+        <v>75</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
@@ -1500,18 +1500,18 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Users visit more often to use rewards</t>
+          <t>% of users who redeem rewards at stores</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Basket Size Uplift</t>
-        </is>
-      </c>
-      <c r="B39" s="12" t="n">
-        <v>8</v>
+          <t>Repeat Visit Increase</t>
+        </is>
+      </c>
+      <c r="B39" s="11" t="n">
+        <v>15</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
@@ -1520,65 +1520,65 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>Users buy more when they have rewards</t>
+          <t>Users visit more often to use rewards</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
+          <t>Basket Size Uplift</t>
+        </is>
+      </c>
+      <c r="B40" s="11" t="n">
+        <v>8</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>%</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Users buy more when they have rewards</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
           <t>Average Basket Value</t>
         </is>
       </c>
-      <c r="B40" s="9" t="n">
+      <c r="B41" s="9" t="n">
         <v>25</v>
       </c>
-      <c r="C40" t="inlineStr">
+      <c r="C41" t="inlineStr">
         <is>
           <t>$</t>
         </is>
       </c>
-      <c r="D40" t="inlineStr">
+      <c r="D41" t="inlineStr">
         <is>
           <t>Typical purchase amount per store visit</t>
         </is>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" s="2" t="inlineStr">
+    <row r="43">
+      <c r="A43" s="2" t="inlineStr">
         <is>
           <t>BRAND BENCHMARKS</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>Meta CPM</t>
-        </is>
-      </c>
-      <c r="B43" s="9" t="n">
-        <v>10</v>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>$</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>Facebook/Instagram ad cost per 1000 impressions</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>TikTok CPM</t>
+          <t>Meta CPM</t>
         </is>
       </c>
       <c r="B44" s="9" t="n">
-        <v>8.5</v>
+        <v>10</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
@@ -1587,25 +1587,45 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>TikTok ad cost per 1000 impressions</t>
+          <t>Facebook/Instagram ad cost per 1000 impressions</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
+          <t>TikTok CPM</t>
+        </is>
+      </c>
+      <c r="B45" s="9" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>$</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>TikTok ad cost per 1000 impressions</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
           <t>Industry Avg CTR</t>
         </is>
       </c>
-      <c r="B45" s="12" t="n">
+      <c r="B46" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="C45" t="inlineStr">
+      <c r="C46" t="inlineStr">
         <is>
           <t>%</t>
         </is>
       </c>
-      <c r="D45" t="inlineStr">
+      <c r="D46" t="inlineStr">
         <is>
           <t>Click-through rate on social media ads (only 1% engage!)</t>
         </is>
@@ -1614,15 +1634,15 @@
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A17:D17"/>
+    <mergeCell ref="A37:D37"/>
+    <mergeCell ref="A18:D18"/>
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A31:D31"/>
+    <mergeCell ref="A12:D12"/>
     <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="A30:D30"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="A24:D24"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="A36:D36"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="A25:D25"/>
+    <mergeCell ref="A43:D43"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -1684,7 +1704,7 @@
         </is>
       </c>
       <c r="B5" s="14">
-        <f>Assumptions!B5*Assumptions!B18/100</f>
+        <f>Assumptions!B5*Assumptions!B19/100</f>
         <v/>
       </c>
       <c r="C5" t="inlineStr">
@@ -1716,7 +1736,7 @@
         </is>
       </c>
       <c r="B7" s="14">
-        <f>B5*Assumptions!B22</f>
+        <f>B5*Assumptions!B23</f>
         <v/>
       </c>
       <c r="C7" t="inlineStr">
@@ -1732,7 +1752,7 @@
         </is>
       </c>
       <c r="B8" s="15">
-        <f>B7*Assumptions!B12</f>
+        <f>B7*Assumptions!B13</f>
         <v/>
       </c>
       <c r="C8" t="inlineStr">
@@ -1764,7 +1784,7 @@
         </is>
       </c>
       <c r="B11" s="15">
-        <f>B7*Assumptions!B13</f>
+        <f>B7*Assumptions!B14</f>
         <v/>
       </c>
       <c r="C11" t="inlineStr">
@@ -1780,7 +1800,7 @@
         </is>
       </c>
       <c r="B12" s="15">
-        <f>B7*Assumptions!B14</f>
+        <f>B7*Assumptions!B15</f>
         <v/>
       </c>
       <c r="C12" t="inlineStr">
@@ -1796,7 +1816,7 @@
         </is>
       </c>
       <c r="B13" s="15">
-        <f>B7*Assumptions!B15</f>
+        <f>B7*Assumptions!B16</f>
         <v/>
       </c>
       <c r="C13" t="inlineStr">
@@ -1851,7 +1871,7 @@
         </is>
       </c>
       <c r="B18">
-        <f>Assumptions!B22</f>
+        <f>Assumptions!B23</f>
         <v/>
       </c>
       <c r="C18" t="inlineStr">
@@ -1867,7 +1887,7 @@
         </is>
       </c>
       <c r="B19" s="19">
-        <f>Assumptions!B22*Assumptions!B12</f>
+        <f>Assumptions!B23*Assumptions!B13</f>
         <v/>
       </c>
       <c r="C19" t="inlineStr">
@@ -1883,7 +1903,7 @@
         </is>
       </c>
       <c r="B20" s="19">
-        <f>Assumptions!B22*(Assumptions!B13+Assumptions!B14)</f>
+        <f>Assumptions!B23*(Assumptions!B14+Assumptions!B15)</f>
         <v/>
       </c>
       <c r="C20" t="inlineStr">
@@ -1899,7 +1919,7 @@
         </is>
       </c>
       <c r="B21" s="19">
-        <f>Assumptions!B22*Assumptions!B15</f>
+        <f>Assumptions!B23*Assumptions!B16</f>
         <v/>
       </c>
       <c r="C21" t="inlineStr">
@@ -1938,7 +1958,7 @@
         </is>
       </c>
       <c r="B25">
-        <f>Assumptions!B21</f>
+        <f>Assumptions!B22</f>
         <v/>
       </c>
       <c r="C25" t="inlineStr">
@@ -1954,7 +1974,7 @@
         </is>
       </c>
       <c r="B26" s="19">
-        <f>Assumptions!B21*Assumptions!B12</f>
+        <f>Assumptions!B22*Assumptions!B13</f>
         <v/>
       </c>
       <c r="C26" t="inlineStr">
@@ -1970,7 +1990,7 @@
         </is>
       </c>
       <c r="B27" s="19">
-        <f>Assumptions!B21*(Assumptions!B13+Assumptions!B14)</f>
+        <f>Assumptions!B22*(Assumptions!B14+Assumptions!B15)</f>
         <v/>
       </c>
       <c r="C27" t="inlineStr">
@@ -2009,7 +2029,7 @@
         </is>
       </c>
       <c r="B31" s="15">
-        <f>B7*(Assumptions!B13+Assumptions!B14)</f>
+        <f>B7*(Assumptions!B14+Assumptions!B15)</f>
         <v/>
       </c>
       <c r="C31" t="inlineStr">
@@ -2025,7 +2045,7 @@
         </is>
       </c>
       <c r="B32" s="15">
-        <f>B31*Assumptions!B37/100</f>
+        <f>B31*Assumptions!B38/100</f>
         <v/>
       </c>
       <c r="C32" t="inlineStr">
@@ -2041,7 +2061,7 @@
         </is>
       </c>
       <c r="B33" s="14">
-        <f>Assumptions!B5*Assumptions!B37/100</f>
+        <f>Assumptions!B5*Assumptions!B38/100</f>
         <v/>
       </c>
       <c r="C33" t="inlineStr">
@@ -2057,7 +2077,7 @@
         </is>
       </c>
       <c r="B34" s="15">
-        <f>B33*Assumptions!B40</f>
+        <f>B33*Assumptions!B41</f>
         <v/>
       </c>
       <c r="C34" t="inlineStr">
@@ -2073,7 +2093,7 @@
         </is>
       </c>
       <c r="B35" s="15">
-        <f>B34*Assumptions!B39/100</f>
+        <f>B34*Assumptions!B40/100</f>
         <v/>
       </c>
       <c r="C35" t="inlineStr">
@@ -2103,7 +2123,7 @@
         </is>
       </c>
       <c r="B39" s="19">
-        <f>Assumptions!B12*1000</f>
+        <f>Assumptions!B13*1000</f>
         <v/>
       </c>
       <c r="C39" t="inlineStr">
@@ -2119,7 +2139,7 @@
         </is>
       </c>
       <c r="B40" s="19">
-        <f>Assumptions!B12</f>
+        <f>Assumptions!B13</f>
         <v/>
       </c>
       <c r="C40" t="inlineStr">
@@ -2158,7 +2178,7 @@
         </is>
       </c>
       <c r="B44" s="19">
-        <f>Assumptions!B43</f>
+        <f>Assumptions!B44</f>
         <v/>
       </c>
       <c r="C44" t="inlineStr">
@@ -2174,7 +2194,7 @@
         </is>
       </c>
       <c r="B45" s="23">
-        <f>Assumptions!B45</f>
+        <f>Assumptions!B46</f>
         <v/>
       </c>
       <c r="C45" t="inlineStr">
@@ -2190,7 +2210,7 @@
         </is>
       </c>
       <c r="B46" s="19">
-        <f>(Assumptions!B43/1000)/(Assumptions!B45/100)</f>
+        <f>(Assumptions!B44/1000)/(Assumptions!B46/100)</f>
         <v/>
       </c>
       <c r="C46" t="inlineStr">
@@ -2626,7 +2646,7 @@
           <t>Avg User Lifetime (months)</t>
         </is>
       </c>
-      <c r="B5" s="12" t="n">
+      <c r="B5" s="11" t="n">
         <v>12</v>
       </c>
       <c r="C5" t="inlineStr">
@@ -2665,7 +2685,7 @@
         </is>
       </c>
       <c r="B9" s="19">
-        <f>B5*Assumptions!B22*Assumptions!B15</f>
+        <f>B5*Assumptions!B23*Assumptions!B16</f>
         <v/>
       </c>
       <c r="C9" t="inlineStr">
@@ -2720,7 +2740,7 @@
         </is>
       </c>
       <c r="B14" s="19">
-        <f>(Assumptions!B4)+(Assumptions!B22*Assumptions!B15)</f>
+        <f>(Assumptions!B4)+(Assumptions!B23*Assumptions!B16)</f>
         <v/>
       </c>
       <c r="C14" t="inlineStr">
@@ -2791,7 +2811,7 @@
         </is>
       </c>
       <c r="B20" s="27">
-        <f>Calculations!B33*12*Assumptions!B40*1.15</f>
+        <f>Calculations!B33*12*Assumptions!B41*1.15</f>
         <v/>
       </c>
       <c r="C20" t="inlineStr">
@@ -3526,7 +3546,7 @@
         </is>
       </c>
       <c r="B22" s="19">
-        <f>-Assumptions!B21*Assumptions!B13</f>
+        <f>-Assumptions!B22*Assumptions!B14</f>
         <v/>
       </c>
       <c r="C22" t="inlineStr">
@@ -3542,7 +3562,7 @@
         </is>
       </c>
       <c r="B23" s="19">
-        <f>-Assumptions!B21*Assumptions!B14</f>
+        <f>-Assumptions!B22*Assumptions!B15</f>
         <v/>
       </c>
       <c r="C23" t="inlineStr">
@@ -3603,7 +3623,7 @@
         </is>
       </c>
       <c r="B39" s="33">
-        <f>(12*(Assumptions!B4+Assumptions!B22*Assumptions!B15))/2</f>
+        <f>(12*(Assumptions!B4+Assumptions!B23*Assumptions!B16))/2</f>
         <v/>
       </c>
       <c r="C39" t="inlineStr">
@@ -3624,7 +3644,7 @@
         </is>
       </c>
       <c r="B40" s="34">
-        <f>2/(Assumptions!B4+Assumptions!B22*Assumptions!B15)</f>
+        <f>2/(Assumptions!B4+Assumptions!B23*Assumptions!B16)</f>
         <v/>
       </c>
       <c r="C40" t="inlineStr">
@@ -3685,7 +3705,7 @@
         </is>
       </c>
       <c r="B45" s="27">
-        <f>Calculations!B31*Assumptions!B37/100</f>
+        <f>Calculations!B31*Assumptions!B38/100</f>
         <v/>
       </c>
       <c r="C45" t="inlineStr">
@@ -3717,7 +3737,7 @@
         </is>
       </c>
       <c r="B47" s="27">
-        <f>Calculations!B34*Assumptions!B39/100</f>
+        <f>Calculations!B34*Assumptions!B40/100</f>
         <v/>
       </c>
       <c r="C47" t="inlineStr">

</xml_diff>